<commit_message>
Minimalized IO-NRF, no Digital Input
</commit_message>
<xml_diff>
--- a/Manufacturing.xlsx
+++ b/Manufacturing.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32-OBD" sheetId="1" r:id="rId1"/>
     <sheet name="ESP32-OBD with IO-NRF" sheetId="3" r:id="rId2"/>
     <sheet name="IO-NRF_minimal (6 db)" sheetId="2" r:id="rId3"/>
+    <sheet name="Beültetési árak" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -196,8 +197,8 @@
   <numFmts count="4">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;Ft&quot;;[Red]\-#,##0\ &quot;Ft&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.0\ &quot;Ft&quot;_-;\-* #,##0.0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0\ &quot;Ft&quot;_-;\-* #,##0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0\ &quot;Ft&quot;_-;\-* #,##0.0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;Ft&quot;_-;\-* #,##0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -324,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -333,7 +334,7 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -619,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1331,4 +1332,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOMs, manufacturing (beültetés árak) and PCBs
</commit_message>
<xml_diff>
--- a/Manufacturing.xlsx
+++ b/Manufacturing.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32-OBD" sheetId="1" r:id="rId1"/>
     <sheet name="ESP32-OBD with IO-NRF" sheetId="3" r:id="rId2"/>
     <sheet name="IO-NRF_minimal (6 db)" sheetId="2" r:id="rId3"/>
     <sheet name="Beültetési árak" sheetId="4" r:id="rId4"/>
+    <sheet name="Összesítő 30 db" sheetId="5" r:id="rId5"/>
+    <sheet name="Teszt gyártás 6 db" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>Tétel neve</t>
   </si>
@@ -188,24 +190,129 @@
   </si>
   <si>
     <t>ár/db (1 db-ra vetítve)</t>
+  </si>
+  <si>
+    <t>IO-NRF minimal</t>
+  </si>
+  <si>
+    <t>Név</t>
+  </si>
+  <si>
+    <t>darabszám</t>
+  </si>
+  <si>
+    <t>Gyártó</t>
+  </si>
+  <si>
+    <t>Méret</t>
+  </si>
+  <si>
+    <t>52x33</t>
+  </si>
+  <si>
+    <t>Darabszám</t>
+  </si>
+  <si>
+    <t>Ajánlott ár</t>
+  </si>
+  <si>
+    <t>Ajánlott ár/db</t>
+  </si>
+  <si>
+    <t>EUR2HUF</t>
+  </si>
+  <si>
+    <t>Ár/db</t>
+  </si>
+  <si>
+    <t>IO-NRF minimal (NO-THT)</t>
+  </si>
+  <si>
+    <t>57x26</t>
+  </si>
+  <si>
+    <t>OBDESP32 (NOTHT)</t>
+  </si>
+  <si>
+    <t>Végösszeg</t>
+  </si>
+  <si>
+    <t>35 SMT, 21 Unique, Double sided</t>
+  </si>
+  <si>
+    <t>22 SMT, 13 Unique, Single sided</t>
+  </si>
+  <si>
+    <t>IO-NRF minimal (THT)</t>
+  </si>
+  <si>
+    <t>ár/db 30 db-ra</t>
+  </si>
+  <si>
+    <t>Tétel név</t>
+  </si>
+  <si>
+    <t>Beültetés (AISLER, EUR)</t>
+  </si>
+  <si>
+    <t>Beültetés (AISLER, HUF)</t>
+  </si>
+  <si>
+    <t>Végösszeg (beültetéssel)</t>
+  </si>
+  <si>
+    <t>Végösszeg/db (beültetéssel)</t>
+  </si>
+  <si>
+    <t>Végösszeg (beültetés nélkül)</t>
+  </si>
+  <si>
+    <t>Végösszeg/db (beültetés nélkül)</t>
+  </si>
+  <si>
+    <t>OBD-ESP32 only</t>
+  </si>
+  <si>
+    <t>30 db ára</t>
+  </si>
+  <si>
+    <t>Alkatrészek + NYÁKgyártás</t>
+  </si>
+  <si>
+    <t>30 db-ra</t>
+  </si>
+  <si>
+    <t>OBD-ESP32 with IO-NRF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="8">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;Ft&quot;;[Red]\-#,##0\ &quot;Ft&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0\ &quot;Ft&quot;_-;\-* #,##0.0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;Ft&quot;_-;\-* #,##0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$Ft-40E]_-;\-* #,##0.00\ [$Ft-40E]_-;_-* &quot;-&quot;??\ [$Ft-40E]_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0.0\ [$Ft-40E]_-;\-* #,##0.0\ [$Ft-40E]_-;_-* &quot;-&quot;??\ [$Ft-40E]_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.0\ [$Ft-40E]_-;\-* #,##0.0\ [$Ft-40E]_-;_-* &quot;-&quot;?\ [$Ft-40E]_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,12 +381,12 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -289,53 +396,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Jó" xfId="2" builtinId="26"/>
@@ -618,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +759,7 @@
     <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -678,7 +800,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -698,7 +820,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -718,7 +840,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -738,7 +860,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -758,7 +880,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -778,8 +900,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="F9">
         <f>6*SUM(F2:F7)</f>
@@ -790,15 +912,18 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>45</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F12">
         <f>F9+G9</f>
         <v>83260</v>
@@ -807,8 +932,12 @@
         <f>SUM(F9+G9)/6</f>
         <v>13876.666666666666</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>F9*5+G9</f>
+        <v>357100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" s="18" t="s">
         <v>46</v>
       </c>
@@ -827,10 +956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +973,7 @@
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -886,7 +1015,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -907,7 +1036,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -928,7 +1057,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -949,7 +1078,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -970,7 +1099,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -991,7 +1120,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -1012,7 +1141,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="8"/>
       <c r="C9" s="3"/>
@@ -1027,10 +1156,10 @@
         <v>16715</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
       <c r="F11" t="s">
         <v>45</v>
@@ -1038,8 +1167,11 @@
       <c r="G11" s="23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="F12">
         <f>F9+G9</f>
@@ -1049,8 +1181,12 @@
         <f>SUM(F9+G9)/6</f>
         <v>14952.833333333334</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>F9*5+G9</f>
+        <v>381725</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" s="18" t="s">
         <v>46</v>
       </c>
@@ -1071,7 +1207,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1429,9 @@
       <c r="I11" s="18" t="s">
         <v>34</v>
       </c>
+      <c r="J11" s="18" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H12" s="10" t="s">
@@ -1300,6 +1439,9 @@
       </c>
       <c r="I12" s="10" t="s">
         <v>42</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1310,6 +1452,10 @@
       <c r="I13" s="17">
         <f>(F2+G2+F3+G3+F6+G6+F7+G7+F9)/6</f>
         <v>11665.06</v>
+      </c>
+      <c r="J13" s="17">
+        <f>(F2+F3+F6+F8+F9)*5/30+SUM(G2:G9)/30</f>
+        <v>11955.226666666666</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1335,6 +1481,403 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="10"/>
+    <col min="5" max="5" width="12" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="10">
+        <v>30</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="24">
+        <v>267.55</v>
+      </c>
+      <c r="F4" s="24">
+        <f>E4/B4</f>
+        <v>8.918333333333333</v>
+      </c>
+      <c r="G4" s="26">
+        <v>395</v>
+      </c>
+      <c r="H4" s="26">
+        <f>F4*G4</f>
+        <v>3522.7416666666663</v>
+      </c>
+      <c r="I4" s="27">
+        <f>H4*B4</f>
+        <v>105682.24999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="10">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="24">
+        <v>161.55000000000001</v>
+      </c>
+      <c r="F5" s="24">
+        <f>E5/B5</f>
+        <v>5.3850000000000007</v>
+      </c>
+      <c r="G5" s="26">
+        <v>395</v>
+      </c>
+      <c r="H5" s="26">
+        <f>F5*G5</f>
+        <v>2127.0750000000003</v>
+      </c>
+      <c r="I5" s="27">
+        <f>H5*B5</f>
+        <v>63812.250000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="10">
+        <v>30</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="24">
+        <v>340.89</v>
+      </c>
+      <c r="F9" s="24">
+        <f>E9/B9</f>
+        <v>11.363</v>
+      </c>
+      <c r="G9" s="26">
+        <v>395</v>
+      </c>
+      <c r="H9" s="26">
+        <f>F9*G9</f>
+        <v>4488.3850000000002</v>
+      </c>
+      <c r="I9" s="27">
+        <f t="shared" ref="I6:I11" si="0">H9*B9</f>
+        <v>134651.55000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="10">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="24">
+        <v>323.93</v>
+      </c>
+      <c r="F10" s="24">
+        <f>E10/B10</f>
+        <v>16.1965</v>
+      </c>
+      <c r="G10" s="26">
+        <v>395</v>
+      </c>
+      <c r="H10" s="26">
+        <f>F10*G10</f>
+        <v>6397.6175000000003</v>
+      </c>
+      <c r="I10" s="27">
+        <f t="shared" si="0"/>
+        <v>127952.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="10">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="24">
+        <v>306.95999999999998</v>
+      </c>
+      <c r="F11" s="24">
+        <f>E11/B11</f>
+        <v>30.695999999999998</v>
+      </c>
+      <c r="G11" s="26">
+        <v>395</v>
+      </c>
+      <c r="H11" s="26">
+        <f>F11*G11</f>
+        <v>12124.92</v>
+      </c>
+      <c r="I11" s="27">
+        <f t="shared" si="0"/>
+        <v>121249.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFB18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12" style="10" customWidth="1"/>
+    <col min="6" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="XFB1" s="10"/>
+    </row>
+    <row r="3" spans="1:9 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="29">
+        <f>11955.22*30</f>
+        <v>358656.6</v>
+      </c>
+      <c r="C3" s="24">
+        <v>161.55000000000001</v>
+      </c>
+      <c r="D3" s="28">
+        <f>C3*E3</f>
+        <v>63812.250000000007</v>
+      </c>
+      <c r="E3" s="10">
+        <v>395</v>
+      </c>
+      <c r="F3" s="25">
+        <f>B3+D3</f>
+        <v>422468.85</v>
+      </c>
+      <c r="G3" s="25">
+        <f>F3/$B$18</f>
+        <v>14082.295</v>
+      </c>
+      <c r="H3" s="29">
+        <f>11955.22*30</f>
+        <v>358656.6</v>
+      </c>
+      <c r="I3" s="25">
+        <f>H3/$B$18</f>
+        <v>11955.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="29">
+        <v>381725</v>
+      </c>
+      <c r="C4" s="24">
+        <v>340.89</v>
+      </c>
+      <c r="D4" s="28">
+        <f>C4*E4</f>
+        <v>134651.54999999999</v>
+      </c>
+      <c r="E4" s="10">
+        <v>395</v>
+      </c>
+      <c r="F4" s="25">
+        <f t="shared" ref="F4:F5" si="0">B4+D4</f>
+        <v>516376.55</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" ref="G4:G5" si="1">F4/$B$18</f>
+        <v>17212.551666666666</v>
+      </c>
+      <c r="H4" s="29">
+        <v>381725</v>
+      </c>
+      <c r="I4" s="25">
+        <f t="shared" ref="I4:I5" si="2">H4/$B$18</f>
+        <v>12724.166666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="26">
+        <v>357100</v>
+      </c>
+      <c r="C5" s="24">
+        <v>340.89</v>
+      </c>
+      <c r="D5" s="28">
+        <f>C5*E5</f>
+        <v>134651.54999999999</v>
+      </c>
+      <c r="E5" s="10">
+        <v>395</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" si="0"/>
+        <v>491751.55</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="1"/>
+        <v>16391.718333333334</v>
+      </c>
+      <c r="H5" s="26">
+        <v>357100</v>
+      </c>
+      <c r="I5" s="25">
+        <f t="shared" si="2"/>
+        <v>11903.333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="10">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>